<commit_message>
Adding Marty's R labs, and Helene's edited version of Lab 3
</commit_message>
<xml_diff>
--- a/EEB319_Lab1_ExcelExample.xlsx
+++ b/EEB319_Lab1_ExcelExample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjarviscross/Desktop/TAing/EEB319/EEB319_PopulationEcology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7E67085C-8700-A44F-ACAC-87E035577E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F4AA6A-011B-8248-970C-6B41AD9D27EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="1680" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{0B991DD1-3D46-6140-9D2F-15F33AB76BBD}"/>
+    <workbookView xWindow="3160" yWindow="1680" windowWidth="28040" windowHeight="17440" xr2:uid="{0B991DD1-3D46-6140-9D2F-15F33AB76BBD}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelDescription" sheetId="4" r:id="rId1"/>
@@ -673,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90697D7-1155-CD4B-A990-CF1690B6EBAC}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31:K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1035,7 +1035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65F25AD9-5DD9-1B42-9B32-7DA07D93B29B}">
   <dimension ref="A1:C502"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>

</xml_diff>